<commit_message>
xinyu update the output excel
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1010,7 +1010,7 @@
         <x:v>12.9</x:v>
       </x:c>
       <x:c r="K2" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>117</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:11">
@@ -1080,7 +1080,7 @@
         <x:v>9.38</x:v>
       </x:c>
       <x:c r="K4" s="0" t="n">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:11">
@@ -1150,7 +1150,7 @@
         <x:v>3.12</x:v>
       </x:c>
       <x:c r="K6" s="0" t="n">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:11">

</xml_diff>

<commit_message>
xinyu connect main with yuxuan and jiale
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -6,10 +6,8 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="a" sheetId="2" r:id="rId2"/>
-    <x:sheet name="b" sheetId="5" r:id="rId5"/>
-    <x:sheet name="c" sheetId="7" r:id="rId7"/>
-    <x:sheet name="d" sheetId="8" r:id="rId8"/>
+    <x:sheet name="KPI for Digital Innovation" sheetId="2" r:id="rId2"/>
+    <x:sheet name="KPI for Procurement" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -40,6 +38,9 @@
     <x:t>AvgComplexity</x:t>
   </x:si>
   <x:si>
+    <x:t>FirstFinalScore</x:t>
+  </x:si>
+  <x:si>
     <x:t>DI0004</x:t>
   </x:si>
   <x:si>
@@ -82,6 +83,9 @@
     <x:t>ErrorRate</x:t>
   </x:si>
   <x:si>
+    <x:t>SecondFinalScore</x:t>
+  </x:si>
+  <x:si>
     <x:t>PE0002</x:t>
   </x:si>
   <x:si>
@@ -101,12 +105,6 @@
   </x:si>
   <x:si>
     <x:t>2025-03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FirstFinalScore</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SecondFinalScore</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -457,13 +455,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G4"/>
+  <x:dimension ref="A1:H4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -485,13 +483,16 @@
       <x:c r="G1" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
         <x:v>6</x:v>
@@ -508,13 +509,16 @@
       <x:c r="G2" s="0" t="n">
         <x:v>1.25</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
+      <x:c r="H2" s="0" t="n">
+        <x:v>73</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8">
       <x:c r="A3" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
         <x:v>6</x:v>
@@ -531,13 +535,16 @@
       <x:c r="G3" s="0" t="n">
         <x:v>1.8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7">
+      <x:c r="H3" s="0" t="n">
+        <x:v>71.4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8">
       <x:c r="A4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
         <x:v>8</x:v>
@@ -553,6 +560,9 @@
       </x:c>
       <x:c r="G4" s="0" t="n">
         <x:v>1.88</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="n">
+        <x:v>93.6666666666667</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -569,374 +579,6 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J7"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:10">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="J1" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:10">
-      <x:c r="A2" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="n">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="n">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="n">
-        <x:v>16380</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="n">
-        <x:v>2761.8</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="n">
-        <x:v>16.86</x:v>
-      </x:c>
-      <x:c r="I2" s="0" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="n">
-        <x:v>12.9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10">
-      <x:c r="A3" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="n">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="n">
-        <x:v>15198</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="n">
-        <x:v>2468.8</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="n">
-        <x:v>16.24</x:v>
-      </x:c>
-      <x:c r="I3" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J3" s="0" t="n">
-        <x:v>3.7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10">
-      <x:c r="A4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="n">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="n">
-        <x:v>14862</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="n">
-        <x:v>2345.1</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="n">
-        <x:v>15.78</x:v>
-      </x:c>
-      <x:c r="I4" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="J4" s="0" t="n">
-        <x:v>9.38</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10">
-      <x:c r="A5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="n">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="n">
-        <x:v>12744</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="n">
-        <x:v>2377.3</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="n">
-        <x:v>18.65</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J5" s="0" t="n">
-        <x:v>3.57</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10">
-      <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="n">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="n">
-        <x:v>18203</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="n">
-        <x:v>2649</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="n">
-        <x:v>14.55</x:v>
-      </x:c>
-      <x:c r="I6" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J6" s="0" t="n">
-        <x:v>3.12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="A7" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="n">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="n">
-        <x:v>14098</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="n">
-        <x:v>2131.9</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="n">
-        <x:v>15.12</x:v>
-      </x:c>
-      <x:c r="I7" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J7" s="0" t="n">
-        <x:v>3.7</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:H4"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:8">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="n">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="n">
-        <x:v>3.25</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="n">
-        <x:v>1.25</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="n">
-        <x:v>73</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="n">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="n">
-        <x:v>4.6</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="n">
-        <x:v>1.8</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="n">
-        <x:v>71.4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="n">
-        <x:v>4.25</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="n">
-        <x:v>1.88</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="n">
-        <x:v>93.6666666666667</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
   <x:dimension ref="A1:K7"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
@@ -951,42 +593,42 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="H1" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="I1" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="J1" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11">
       <x:c r="A2" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
         <x:v>31</x:v>
@@ -1015,13 +657,13 @@
     </x:row>
     <x:row r="3" spans="1:11">
       <x:c r="A3" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
         <x:v>27</x:v>
@@ -1050,13 +692,13 @@
     </x:row>
     <x:row r="4" spans="1:11">
       <x:c r="A4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
         <x:v>32</x:v>
@@ -1085,13 +727,13 @@
     </x:row>
     <x:row r="5" spans="1:11">
       <x:c r="A5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
         <x:v>28</x:v>
@@ -1120,13 +762,13 @@
     </x:row>
     <x:row r="6" spans="1:11">
       <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
         <x:v>32</x:v>
@@ -1155,13 +797,13 @@
     </x:row>
     <x:row r="7" spans="1:11">
       <x:c r="A7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
         <x:v>27</x:v>

</xml_diff>